<commit_message>
update the test result
</commit_message>
<xml_diff>
--- a/3_Result.xlsx
+++ b/3_Result.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAP\SAP_Projects\SME\SME WIP\Ramp-up Plan\Ramp-up Sessions\03. Node.js New Features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAP\SAP_Projects\SME\SME WIP\Ramp-up Plan\Status Tracking\Team-Ramp-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D9DDAB-3D56-49AB-A0D7-C8B1373B556C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1718FBDB-836F-4982-A76B-561C7EDBF4E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7560"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet名称" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -419,9 +412,6 @@
     <t>`2019-08-23 13:40:28</t>
   </si>
   <si>
-    <t>`50分</t>
-  </si>
-  <si>
     <t>`28</t>
   </si>
   <si>
@@ -518,9 +508,6 @@
     <t>`1分45秒</t>
   </si>
   <si>
-    <t>`30分</t>
-  </si>
-  <si>
     <t>`36</t>
   </si>
   <si>
@@ -546,12 +533,18 @@
   </si>
   <si>
     <t>`3分22秒</t>
+  </si>
+  <si>
+    <t>`100分</t>
+  </si>
+  <si>
+    <t>`40分</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -579,7 +572,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
   </cellXfs>
@@ -895,11 +889,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -911,14 +905,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -957,7 +951,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -976,8 +970,8 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
+      <c r="F4" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -997,7 +991,7 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1016,8 +1010,8 @@
       <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
-        <v>22</v>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1036,8 +1030,8 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1056,8 +1050,8 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" t="s">
-        <v>22</v>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1076,8 +1070,8 @@
       <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -1096,8 +1090,8 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -1116,8 +1110,8 @@
       <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
-        <v>22</v>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -1136,8 +1130,8 @@
       <c r="E12" t="s">
         <v>54</v>
       </c>
-      <c r="F12" t="s">
-        <v>22</v>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1156,8 +1150,8 @@
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -1176,8 +1170,8 @@
       <c r="E14" t="s">
         <v>63</v>
       </c>
-      <c r="F14" t="s">
-        <v>22</v>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1196,8 +1190,8 @@
       <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" t="s">
-        <v>22</v>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -1217,7 +1211,7 @@
         <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -1236,8 +1230,8 @@
       <c r="E17" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
-        <v>73</v>
+      <c r="F17" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1256,8 +1250,8 @@
       <c r="E18" t="s">
         <v>81</v>
       </c>
-      <c r="F18" t="s">
-        <v>73</v>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1276,8 +1270,8 @@
       <c r="E19" t="s">
         <v>85</v>
       </c>
-      <c r="F19" t="s">
-        <v>73</v>
+      <c r="F19" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1296,8 +1290,8 @@
       <c r="E20" t="s">
         <v>89</v>
       </c>
-      <c r="F20" t="s">
-        <v>73</v>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1316,8 +1310,8 @@
       <c r="E21" t="s">
         <v>93</v>
       </c>
-      <c r="F21" t="s">
-        <v>73</v>
+      <c r="F21" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -1336,8 +1330,8 @@
       <c r="E22" t="s">
         <v>98</v>
       </c>
-      <c r="F22" t="s">
-        <v>73</v>
+      <c r="F22" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1356,8 +1350,8 @@
       <c r="E23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" t="s">
-        <v>73</v>
+      <c r="F23" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -1376,8 +1370,8 @@
       <c r="E24" t="s">
         <v>106</v>
       </c>
-      <c r="F24" t="s">
-        <v>73</v>
+      <c r="F24" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -1396,8 +1390,8 @@
       <c r="E25" t="s">
         <v>111</v>
       </c>
-      <c r="F25" t="s">
-        <v>73</v>
+      <c r="F25" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -1416,8 +1410,8 @@
       <c r="E26" t="s">
         <v>115</v>
       </c>
-      <c r="F26" t="s">
-        <v>73</v>
+      <c r="F26" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -1437,7 +1431,7 @@
         <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -1456,8 +1450,8 @@
       <c r="E28" t="s">
         <v>125</v>
       </c>
-      <c r="F28" t="s">
-        <v>121</v>
+      <c r="F28" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -1477,78 +1471,78 @@
         <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" t="s">
         <v>131</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>132</v>
-      </c>
-      <c r="C30" t="s">
-        <v>133</v>
       </c>
       <c r="D30" t="s">
         <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>134</v>
-      </c>
-      <c r="F30" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" t="s">
         <v>135</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>136</v>
-      </c>
-      <c r="C31" t="s">
-        <v>137</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
         <v>139</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>140</v>
-      </c>
-      <c r="C32" t="s">
-        <v>141</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>142</v>
-      </c>
-      <c r="F32" t="s">
-        <v>130</v>
+        <v>141</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
         <v>143</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>144</v>
-      </c>
-      <c r="C33" t="s">
-        <v>145</v>
       </c>
       <c r="D33" t="s">
         <v>26</v>
@@ -1556,128 +1550,128 @@
       <c r="E33" t="s">
         <v>50</v>
       </c>
-      <c r="F33" t="s">
-        <v>130</v>
+      <c r="F33" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" t="s">
         <v>146</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>147</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>148</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>149</v>
       </c>
-      <c r="E34" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" t="s">
-        <v>130</v>
+      <c r="F34" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" t="s">
         <v>151</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>152</v>
-      </c>
-      <c r="C35" t="s">
-        <v>153</v>
       </c>
       <c r="D35" t="s">
         <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>154</v>
-      </c>
-      <c r="F35" t="s">
-        <v>130</v>
+        <v>153</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" t="s">
         <v>155</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>156</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" t="s">
         <v>157</v>
       </c>
-      <c r="D36" t="s">
-        <v>149</v>
-      </c>
-      <c r="E36" t="s">
-        <v>158</v>
-      </c>
-      <c r="F36" t="s">
-        <v>130</v>
+      <c r="F36" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" t="s">
         <v>159</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>160</v>
-      </c>
-      <c r="C37" t="s">
-        <v>161</v>
       </c>
       <c r="D37" t="s">
         <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F37" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" t="s">
         <v>164</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>165</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>166</v>
       </c>
-      <c r="D38" t="s">
-        <v>167</v>
-      </c>
-      <c r="E38" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" t="s">
-        <v>163</v>
+      <c r="F38" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" t="s">
         <v>169</v>
-      </c>
-      <c r="B39" t="s">
-        <v>170</v>
-      </c>
-      <c r="C39" t="s">
-        <v>171</v>
       </c>
       <c r="D39" t="s">
         <v>16</v>
       </c>
       <c r="E39" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F39" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1686,7 +1680,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>